<commit_message>
Made some minor checks in my calculations. Not sure where the errors are
</commit_message>
<xml_diff>
--- a/HW_2_2_2.xlsx
+++ b/HW_2_2_2.xlsx
@@ -338,16 +338,7 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -364,11 +355,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="96" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,10 +659,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="15"/>
       <c r="M1" t="s">
         <v>26</v>
       </c>
@@ -716,10 +716,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="15"/>
       <c r="K2" t="s">
         <v>20</v>
       </c>
@@ -795,15 +795,15 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="17">
         <v>44081</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="17"/>
       <c r="L3">
         <v>3</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:R17" si="0">4*$B$7/(PI()*$L3)*SINH($L3*PI()*$C$30/$E$19)*SIN($L3*PI()*$B$30/$E$19)/(SINH($L3*PI()*$E$19/$E$19))</f>
+        <f t="shared" ref="M3:M17" si="0">4*$B$7/(PI()*$L3)*SINH($L3*PI()*$C$30/$E$19)*SIN($L3*PI()*$B$30/$E$19)/(SINH($L3*PI()*$E$19/$E$19))</f>
         <v>2.2469826291753116E-16</v>
       </c>
       <c r="N3">
@@ -823,7 +823,7 @@
         <v>1.7975861033402492E-16</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S2:U17" si="5">4*$B$8/(PI()*$L3)*SINH($L3*PI()*$C$30/$E$19)*SIN($L3*PI()*$B$30/$E$19)/(SINH($L3*PI()*$E$19/$E$19))</f>
+        <f t="shared" ref="S3:U17" si="5">4*$B$8/(PI()*$L3)*SINH($L3*PI()*$C$30/$E$19)*SIN($L3*PI()*$B$30/$E$19)/(SINH($L3*PI()*$E$19/$E$19))</f>
         <v>1.7975861033402492E-16</v>
       </c>
       <c r="T3">
@@ -839,7 +839,7 @@
         <v>4.4939652583506231E-17</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X2:Z17" si="7">4*$B$9/(PI()*$L3)*SINH($L3*PI()*$C$30/$E$19)*SIN($L3*PI()*$B$30/$E$19)/(SINH($L3*PI()*$E$19/$E$19))</f>
+        <f t="shared" ref="X3:Z17" si="7">4*$B$9/(PI()*$L3)*SINH($L3*PI()*$C$30/$E$19)*SIN($L3*PI()*$B$30/$E$19)/(SINH($L3*PI()*$E$19/$E$19))</f>
         <v>4.4939652583506231E-17</v>
       </c>
       <c r="Y3">
@@ -855,7 +855,7 @@
         <v>1.3481895775051871E-16</v>
       </c>
       <c r="AC3">
-        <f t="shared" ref="AC2:AE17" si="9">4*$B$10/(PI()*$L3)*SINH($L3*PI()*$C$30/$E$19)*SIN($L3*PI()*$B$30/$E$19)/(SINH($L3*PI()*$E$19/$E$19))</f>
+        <f t="shared" ref="AC3:AE17" si="9">4*$B$10/(PI()*$L3)*SINH($L3*PI()*$C$30/$E$19)*SIN($L3*PI()*$B$30/$E$19)/(SINH($L3*PI()*$E$19/$E$19))</f>
         <v>1.3481895775051871E-16</v>
       </c>
       <c r="AD3">
@@ -871,10 +871,10 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="15"/>
       <c r="L4">
         <v>5</v>
       </c>
@@ -1013,10 +1013,10 @@
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="15"/>
       <c r="L6">
         <v>9</v>
       </c>
@@ -1092,12 +1092,12 @@
       <c r="B7">
         <v>100</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
       <c r="L7">
         <v>11</v>
       </c>
@@ -1173,10 +1173,10 @@
       <c r="B8">
         <v>80</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
       <c r="L8">
         <v>13</v>
       </c>
@@ -1252,10 +1252,10 @@
       <c r="B9">
         <v>20</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
       <c r="L9">
         <v>15</v>
       </c>
@@ -1331,10 +1331,10 @@
       <c r="B10">
         <v>60</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="L10">
         <v>17</v>
       </c>
@@ -1633,34 +1633,34 @@
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="4">
         <f>AVERAGE($B$7,$B$11,$B$11,$B$8)</f>
         <v>77.5</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="4">
         <f>AVERAGE($B$7,B$15,B$16,$B$8)</f>
         <v>79.0625</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="4">
         <f t="shared" ref="D14:H14" si="10">AVERAGE($B$7,C$15,C$16,$B$8)</f>
         <v>77.890625</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="4">
         <f t="shared" si="10"/>
         <v>77.59765625</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="4">
         <f t="shared" si="10"/>
         <v>77.5244140625</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="4">
         <f t="shared" si="10"/>
         <v>77.506103515625</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="5">
         <f t="shared" si="10"/>
         <v>77.50152587890625</v>
       </c>
@@ -1733,34 +1733,34 @@
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="7">
         <f>AVERAGE($B$7,$B$9,$B$11,B$14)</f>
         <v>65.625</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <f>AVERAGE($B$7,$B$9,B$17,C$14)</f>
         <v>63.28125</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="7">
         <f t="shared" ref="D15:H15" si="11">AVERAGE($B$7,$B$9,C$17,D$14)</f>
         <v>62.6953125</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="7">
         <f t="shared" si="11"/>
         <v>62.548828125</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15" s="7">
         <f t="shared" si="11"/>
         <v>62.51220703125</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="7">
         <f t="shared" si="11"/>
         <v>62.5030517578125</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="8">
         <f t="shared" si="11"/>
         <v>62.500762939453125</v>
       </c>
@@ -1833,34 +1833,34 @@
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="7">
         <f>AVERAGE(B$14,$B$11,$B$10,$B$8)</f>
         <v>70.625</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <f>AVERAGE(C$14,B$17,$B$10,$B$8)</f>
         <v>68.28125</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="7">
         <f t="shared" ref="D16:H16" si="12">AVERAGE(D$14,C$17,$B$10,$B$8)</f>
         <v>67.6953125</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="7">
         <f t="shared" si="12"/>
         <v>67.548828125</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16" s="7">
         <f t="shared" si="12"/>
         <v>67.51220703125</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="7">
         <f t="shared" si="12"/>
         <v>67.5030517578125</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="8">
         <f t="shared" si="12"/>
         <v>67.500762939453125</v>
       </c>
@@ -1933,34 +1933,34 @@
       </c>
     </row>
     <row r="17" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="10">
         <f>AVERAGE(B$15,$B$9,$B$10,B$16)</f>
         <v>54.0625</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="10">
         <f>AVERAGE(C$15,$B$9,$B$10,C$16)</f>
         <v>52.890625</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="10">
         <f t="shared" ref="D17:H17" si="13">AVERAGE(D$15,$B$9,$B$10,D$16)</f>
         <v>52.59765625</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="10">
         <f t="shared" si="13"/>
         <v>52.5244140625</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <f t="shared" si="13"/>
         <v>52.506103515625</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="10">
         <f t="shared" si="13"/>
         <v>52.50152587890625</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="11">
         <f t="shared" si="13"/>
         <v>52.500381469726562</v>
       </c>
@@ -2110,51 +2110,51 @@
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B20">
         <v>75.2</v>
       </c>
-      <c r="N20" s="15" t="s">
+      <c r="N20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B21">
         <v>60.5</v>
       </c>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B22">
         <v>65.400000000000006</v>
       </c>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B23">
@@ -2162,21 +2162,21 @@
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="1" t="s">
+      <c r="C25" s="18"/>
+      <c r="D25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B26" t="e">
@@ -2185,40 +2185,40 @@
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="18" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="I29" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B30">
@@ -2231,16 +2231,16 @@
         <f>SUM(M$18,R$18,W$18,AB$18)</f>
         <v>77.986627653439228</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B31">
@@ -2250,19 +2250,19 @@
         <v>2</v>
       </c>
       <c r="E31">
-        <f t="shared" ref="E30:G33" si="24">SUM(N$18,S$18,X$18,AC$18)</f>
+        <f t="shared" ref="E31:G33" si="24">SUM(N$18,S$18,X$18,AC$18)</f>
         <v>62.23652494532859</v>
       </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B32">
@@ -2275,16 +2275,16 @@
         <f t="shared" si="24"/>
         <v>67.593065286483125</v>
       </c>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B33">
@@ -2297,81 +2297,81 @@
         <f t="shared" si="24"/>
         <v>46.592928342335618</v>
       </c>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="N20:S22"/>
     <mergeCell ref="D7:G10"/>
     <mergeCell ref="I29:O39"/>
     <mergeCell ref="D25:I25"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="D28:G29"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="B25:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>